<commit_message>
2.3.4: [Java] Now generics are fully parsed and imported appropriately.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoCgTypeObject.xlsx
+++ b/meta/program/BlancoCgTypeObject.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoCg/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D059349-A79A-884A-A9E6-6416ADE934DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD4BF54-E12F-A54B-82A0-3C0E81267C4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="640"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -293,6 +293,64 @@
     </rPh>
     <rPh sb="39" eb="41">
       <t xml:space="preserve">キジュツ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>genericsList</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>java.util.List&lt;java.lang.String&gt;</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>new java.util.ArrayList&lt;&gt;()</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>K, Vなど複数のジェネリクスを追加する場合はこちらを使用します。</t>
+    <rPh sb="6" eb="8">
+      <t xml:space="preserve">フクスウ </t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t xml:space="preserve">ツイカ </t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t xml:space="preserve">バアイハ </t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t xml:space="preserve">シヨウシマス。 </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>genericsTree</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>java.util.List&lt;blanco.cg.valueobject.BlancoCgType&gt;</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>v2.4.4 以降で有効なジェネリクスの解析機能を使用するために用います。</t>
+    <rPh sb="7" eb="9">
+      <t xml:space="preserve">イコウ </t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t xml:space="preserve">ユウコウナ </t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t xml:space="preserve">カイセキ </t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t xml:space="preserve">キノウ </t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t xml:space="preserve">シヨウスル </t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t xml:space="preserve">モチイマス </t>
     </rPh>
     <phoneticPr fontId="4"/>
   </si>
@@ -300,7 +358,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -1142,14 +1200,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1435,7 +1493,7 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="21">
-        <f>A28+1</f>
+        <f t="shared" ref="A29:A34" si="0">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="22" t="s">
@@ -1452,66 +1510,104 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="21">
-        <f>A29+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="D30" s="44" t="s">
-        <v>44</v>
+        <v>52</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>53</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="F30" s="25"/>
     </row>
-    <row r="31" spans="1:6" ht="43.5" customHeight="1">
+    <row r="31" spans="1:6">
       <c r="A31" s="21">
-        <f>A30+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="F31" s="51"/>
+        <v>56</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F31" s="25"/>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="21">
-        <f>A31+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B32" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" s="25"/>
+    </row>
+    <row r="33" spans="1:6" ht="43.5" customHeight="1">
+      <c r="A33" s="21">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B33" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="F33" s="51"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="21">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B34" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="23" t="s">
+      <c r="C34" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="23"/>
-      <c r="E32" s="24" t="s">
+      <c r="D34" s="23"/>
+      <c r="E34" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="F32" s="25"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="26"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="29"/>
+      <c r="F34" s="25"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="26"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -1524,30 +1620,30 @@
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="C8:F8"/>
-    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E33:F33"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="E25:E26"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D49">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D51" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>adjustDefaultValue</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>createToString</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>accessScope2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>isAbstract</formula1>
     </dataValidation>
   </dataValidations>
@@ -1560,7 +1656,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>

<commit_message>
2.3.5: [kotlin] Enable to specific generics to extends class.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoCgTypeObject.xlsx
+++ b/meta/program/BlancoCgTypeObject.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoCg/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD4BF54-E12F-A54B-82A0-3C0E81267C4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADCEC06-FF45-CE45-A89A-0E6C1AB74857}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -297,31 +297,7 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>genericsList</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>java.util.List&lt;java.lang.String&gt;</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>new java.util.ArrayList&lt;&gt;()</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>K, Vなど複数のジェネリクスを追加する場合はこちらを使用します。</t>
-    <rPh sb="6" eb="8">
-      <t xml:space="preserve">フクスウ </t>
-    </rPh>
-    <rPh sb="16" eb="18">
-      <t xml:space="preserve">ツイカ </t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t xml:space="preserve">バアイハ </t>
-    </rPh>
-    <rPh sb="27" eb="29">
-      <t xml:space="preserve">シヨウシマス。 </t>
-    </rPh>
     <phoneticPr fontId="4"/>
   </si>
   <si>
@@ -851,12 +827,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -879,12 +861,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1204,10 +1180,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1274,12 +1250,12 @@
         <v>12</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="49"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="51"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="17" t="s">
@@ -1380,23 +1356,23 @@
       <c r="F18"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="55" t="s">
+      <c r="A19" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="56" t="s">
+      <c r="B19" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="54"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="56"/>
       <c r="F19"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="55"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="54"/>
+      <c r="A20" s="45"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="56"/>
       <c r="F20"/>
     </row>
     <row r="21" spans="1:6">
@@ -1433,29 +1409,29 @@
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A25" s="55" t="s">
+      <c r="A25" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="55" t="s">
+      <c r="B25" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="45" t="s">
+      <c r="C25" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="45" t="s">
+      <c r="D25" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="45" t="s">
+      <c r="E25" s="48" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="30"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="55"/>
-      <c r="B26" s="55"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
+      <c r="A26" s="45"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
       <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:6" ht="55.25" customHeight="1">
@@ -1469,10 +1445,10 @@
         <v>35</v>
       </c>
       <c r="D27" s="20"/>
-      <c r="E27" s="52" t="s">
+      <c r="E27" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="F27" s="53"/>
+      <c r="F27" s="55"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="21">
@@ -1493,7 +1469,7 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="21">
-        <f t="shared" ref="A29:A34" si="0">A28+1</f>
+        <f t="shared" ref="A29:A33" si="0">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="22" t="s">
@@ -1514,13 +1490,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="23" t="s">
         <v>51</v>
-      </c>
-      <c r="C30" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30" s="23" t="s">
-        <v>53</v>
       </c>
       <c r="E30" s="23" t="s">
         <v>54</v>
@@ -1533,101 +1509,82 @@
         <v>5</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="D31" s="23" t="s">
-        <v>53</v>
+        <v>39</v>
+      </c>
+      <c r="D31" s="44" t="s">
+        <v>44</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="F31" s="25"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" ht="43.5" customHeight="1">
       <c r="A32" s="21">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D32" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="E32" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="F32" s="25"/>
-    </row>
-    <row r="33" spans="1:6" ht="43.5" customHeight="1">
+        <v>46</v>
+      </c>
+      <c r="E32" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="F32" s="53"/>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="21">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="D33" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="E33" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="F33" s="51"/>
+        <v>35</v>
+      </c>
+      <c r="D33" s="23"/>
+      <c r="E33" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33" s="25"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="21">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B34" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="D34" s="23"/>
-      <c r="E34" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="F34" s="25"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="26"/>
-      <c r="B35" s="27"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="29"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E25:E26"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E25:E26"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D51" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D50" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>